<commit_message>
Minor changes getting ready to create application
</commit_message>
<xml_diff>
--- a/EmployeeData/EmployeeData.xlsx
+++ b/EmployeeData/EmployeeData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8900" windowHeight="6090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20620" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>